<commit_message>
conduct S3 tests for GraphQL and GraphQL with selected fields
</commit_message>
<xml_diff>
--- a/Wyniki 3/S2.xlsx
+++ b/Wyniki 3/S2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A156B6-D7E2-4F55-B9E3-FAC12688BBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28FB694-1F9C-4F9B-9683-CC44786AF69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REST" sheetId="1" r:id="rId1"/>
@@ -1072,20 +1072,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E7:K50"/>
+  <dimension ref="E7:R50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.7265625" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,891 +1119,1101 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E9" s="8">
         <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="N9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="N10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="N11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="N12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="N13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="Q13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="R13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="N15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="N16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="N17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="N18" s="1">
         <v>167502</v>
       </c>
-      <c r="H18" s="1">
+      <c r="O18" s="1">
         <v>167514</v>
       </c>
-      <c r="I18" s="1">
+      <c r="P18" s="1">
         <v>167474</v>
       </c>
-      <c r="J18" s="3">
+      <c r="Q18" s="3">
         <v>167494</v>
       </c>
-      <c r="K18" s="3">
+      <c r="R18" s="3">
         <v>167494</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="N19" s="1">
         <v>960.2</v>
       </c>
-      <c r="H19" s="1">
+      <c r="O19" s="1">
         <v>960.1</v>
       </c>
-      <c r="I19" s="1">
+      <c r="P19" s="1">
         <v>960.2</v>
       </c>
-      <c r="J19" s="3">
+      <c r="Q19" s="3">
         <v>960.2</v>
       </c>
-      <c r="K19" s="3">
+      <c r="R19" s="3">
         <v>960.3</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="N20" s="1">
         <v>174.44</v>
       </c>
-      <c r="H20" s="1">
+      <c r="O20" s="1">
         <v>174.47</v>
       </c>
-      <c r="I20" s="1">
+      <c r="P20" s="1">
         <v>174.41</v>
       </c>
-      <c r="J20" s="3">
+      <c r="Q20" s="3">
         <v>174.44</v>
       </c>
-      <c r="K20" s="3">
+      <c r="R20" s="3">
         <v>174.41</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="N21" s="1">
         <v>15</v>
       </c>
-      <c r="H21" s="1">
+      <c r="O21" s="1">
         <v>15</v>
       </c>
-      <c r="I21" s="1">
+      <c r="P21" s="1">
         <v>15</v>
       </c>
-      <c r="J21" s="3">
+      <c r="Q21" s="3">
         <v>15</v>
       </c>
-      <c r="K21" s="3">
+      <c r="R21" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="N22" s="1">
         <v>17</v>
       </c>
-      <c r="H22" s="1">
+      <c r="O22" s="1">
         <v>17</v>
       </c>
-      <c r="I22" s="1">
+      <c r="P22" s="1">
         <v>17</v>
       </c>
-      <c r="J22" s="3">
+      <c r="Q22" s="3">
         <v>17</v>
       </c>
-      <c r="K22" s="3">
+      <c r="R22" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="N23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="O23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="Q23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="R23" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="N24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="Q24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="R24" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="N25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="O25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="Q25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="R25" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="N26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="P26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="Q26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="R26" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="N27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="P27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="Q27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="R27" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="N28" s="2">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>0</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="N29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="P29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="R29" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="N30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="P30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="Q30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="R30" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="N31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="O31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="P31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="Q31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="R31" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="N32" s="2">
         <v>508888</v>
       </c>
-      <c r="H32" s="2">
+      <c r="O32" s="2">
         <v>507826</v>
       </c>
-      <c r="I32" s="2">
+      <c r="P32" s="2">
         <v>508070</v>
       </c>
-      <c r="J32" s="4">
+      <c r="Q32" s="4">
         <v>511162</v>
       </c>
-      <c r="K32" s="4">
+      <c r="R32" s="4">
         <v>510544</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="N33" s="2">
         <v>960.6</v>
       </c>
-      <c r="H33" s="2">
+      <c r="O33" s="2">
         <v>960.9</v>
       </c>
-      <c r="I33" s="2">
+      <c r="P33" s="2">
         <v>961</v>
       </c>
-      <c r="J33" s="4">
+      <c r="Q33" s="4">
         <v>961</v>
       </c>
-      <c r="K33" s="4">
+      <c r="R33" s="4">
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="N34" s="2">
         <v>529.77</v>
       </c>
-      <c r="H34" s="2">
+      <c r="O34" s="2">
         <v>528.5</v>
       </c>
-      <c r="I34" s="2">
+      <c r="P34" s="2">
         <v>528.70000000000005</v>
       </c>
-      <c r="J34" s="4">
+      <c r="Q34" s="4">
         <v>531.9</v>
       </c>
-      <c r="K34" s="4">
+      <c r="R34" s="4">
         <v>531.59</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="N35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="O35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="P35" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="Q35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="R35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="N36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="O36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="P36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="Q36" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="R36" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="N37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="R37" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="N38" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="P38" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="Q38" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="N39" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="P39" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="N40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="P40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="Q40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="N41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="Q41" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K41" s="3" t="s">
+      <c r="R41" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0</v>
-      </c>
-      <c r="J42" s="3">
-        <v>0</v>
-      </c>
-      <c r="K42" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="N42" s="1">
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>0</v>
+      </c>
+      <c r="R42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="N43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="P43" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="Q43" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="K43" s="3" t="s">
+      <c r="R43" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="N44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="P44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="Q44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="R44" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="N45" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="P45" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J45" s="3" t="s">
+      <c r="Q45" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="R45" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="N46" s="1">
         <v>518326</v>
       </c>
-      <c r="H46" s="1">
+      <c r="O46" s="1">
         <v>519778</v>
       </c>
-      <c r="I46" s="1">
+      <c r="P46" s="1">
         <v>518252</v>
       </c>
-      <c r="J46" s="3">
+      <c r="Q46" s="3">
         <v>522124</v>
       </c>
-      <c r="K46" s="3">
+      <c r="R46" s="3">
         <v>521958</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="N47" s="1">
         <v>960.7</v>
       </c>
-      <c r="H47" s="1">
+      <c r="O47" s="1">
         <v>960.5</v>
       </c>
-      <c r="I47" s="1">
+      <c r="P47" s="1">
         <v>960.6</v>
       </c>
-      <c r="J47" s="3">
+      <c r="Q47" s="3">
         <v>960.8</v>
       </c>
-      <c r="K47" s="3">
+      <c r="R47" s="3">
         <v>960.8</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="N48" s="1">
         <v>539.52</v>
       </c>
-      <c r="H48" s="1">
+      <c r="O48" s="1">
         <v>541.15</v>
       </c>
-      <c r="I48" s="1">
+      <c r="P48" s="1">
         <v>539.52</v>
       </c>
-      <c r="J48" s="3">
+      <c r="Q48" s="3">
         <v>543.41999999999996</v>
       </c>
-      <c r="K48" s="3">
+      <c r="R48" s="3">
         <v>543.26</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="N49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="P49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="Q49" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="R49" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="N50" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="P50" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="Q50" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="K50" s="3" t="s">
+      <c r="R50" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2022,18 +2232,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E427240-8CAA-40AB-9EE3-C007F0D8C5C2}">
   <dimension ref="E7:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.7265625" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="5" t="s">
         <v>158</v>
       </c>
@@ -2044,7 +2254,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2067,7 +2277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -2090,7 +2300,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -2111,7 +2321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -2132,7 +2342,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -2153,7 +2363,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -2174,7 +2384,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -2195,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -2216,7 +2426,7 @@
         <v>42.68</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -2237,7 +2447,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -2258,7 +2468,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -2279,7 +2489,7 @@
         <v>83926</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -2300,7 +2510,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -2321,7 +2531,7 @@
         <v>87.42</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -2342,7 +2552,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2363,7 +2573,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -2386,7 +2596,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -2407,7 +2617,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -2428,7 +2638,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -2449,7 +2659,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -2470,7 +2680,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -2491,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -2512,7 +2722,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -2533,7 +2743,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -2554,7 +2764,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -2575,7 +2785,7 @@
         <v>839084</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -2596,7 +2806,7 @@
         <v>960.7</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -2617,7 +2827,7 @@
         <v>873.39</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -2638,7 +2848,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -2659,7 +2869,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -2682,7 +2892,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -2703,7 +2913,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -2724,7 +2934,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -2745,7 +2955,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -2766,7 +2976,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -2787,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -2808,7 +3018,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -2829,7 +3039,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -2850,7 +3060,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -2871,7 +3081,7 @@
         <v>2129167</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -2892,7 +3102,7 @@
         <v>960.8</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -2913,7 +3123,7 @@
         <v>2216.09</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -2934,7 +3144,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -2974,14 +3184,14 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.7265625" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2992,7 +3202,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -3015,7 +3225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -3038,7 +3248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -3059,7 +3269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -3080,7 +3290,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -3101,7 +3311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -3122,7 +3332,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -3143,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -3164,7 +3374,7 @@
         <v>43.13</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -3185,7 +3395,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -3206,7 +3416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -3227,7 +3437,7 @@
         <v>83888</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -3248,7 +3458,7 @@
         <v>960.6</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -3269,7 +3479,7 @@
         <v>87.33</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -3290,7 +3500,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -3311,7 +3521,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -3334,7 +3544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -3355,7 +3565,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -3376,7 +3586,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -3397,7 +3607,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -3418,7 +3628,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -3439,7 +3649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -3460,7 +3670,7 @@
         <v>142.69999999999999</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -3481,7 +3691,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -3502,7 +3712,7 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -3523,7 +3733,7 @@
         <v>838800</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -3544,7 +3754,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -3565,7 +3775,7 @@
         <v>873.34</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -3586,7 +3796,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -3607,7 +3817,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -3630,7 +3840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -3651,7 +3861,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -3672,7 +3882,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -3693,7 +3903,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -3714,7 +3924,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -3735,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -3756,7 +3966,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -3777,7 +3987,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -3798,7 +4008,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -3819,7 +4029,7 @@
         <v>1642210</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -3840,7 +4050,7 @@
         <v>960.6</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -3861,7 +4071,7 @@
         <v>1709.57</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -3882,7 +4092,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -3918,18 +4128,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33E3BDB-BD67-41A1-991C-2FB34B0212C5}">
   <dimension ref="E7:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="33.7265625" customWidth="1"/>
-    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E7" s="5" t="s">
         <v>72</v>
       </c>
@@ -3940,7 +4150,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -3963,7 +4173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -3986,7 +4196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -4007,7 +4217,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -4028,7 +4238,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -4049,7 +4259,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -4070,7 +4280,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -4091,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -4112,7 +4322,7 @@
         <v>42.53</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -4133,7 +4343,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -4154,7 +4364,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -4175,7 +4385,7 @@
         <v>83889</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -4196,7 +4406,7 @@
         <v>960.5</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -4217,7 +4427,7 @@
         <v>87.34</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -4238,7 +4448,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -4259,7 +4469,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -4282,7 +4492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -4303,7 +4513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -4324,7 +4534,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -4345,7 +4555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -4366,7 +4576,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -4387,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -4408,7 +4618,7 @@
         <v>42.03</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -4429,7 +4639,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -4450,7 +4660,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -4471,7 +4681,7 @@
         <v>838747</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -4492,7 +4702,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -4513,7 +4723,7 @@
         <v>873.32</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -4534,7 +4744,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -4555,7 +4765,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -4578,7 +4788,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -4599,7 +4809,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -4620,7 +4830,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -4641,7 +4851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -4662,7 +4872,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -4683,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -4704,7 +4914,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -4725,7 +4935,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -4746,7 +4956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -4767,7 +4977,7 @@
         <v>1707670</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -4788,7 +4998,7 @@
         <v>960.5</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -4809,7 +5019,7 @@
         <v>1777.84</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -4830,7 +5040,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
create second version of Graphql api
</commit_message>
<xml_diff>
--- a/Wyniki 3/S2.xlsx
+++ b/Wyniki 3/S2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E801E9C-2DBF-4662-B28A-FEBF6FDD24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC57E55C-7A8D-484B-A409-6D4A8F76E003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REST" sheetId="1" r:id="rId1"/>
@@ -1660,19 +1660,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E7:R50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44:L49"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
-    <col min="7" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="7" max="11" width="9.81640625" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -1780,7 +1780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -1816,7 +1816,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -1852,7 +1852,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -1888,7 +1888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -1960,7 +1960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -1996,7 +1996,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -2032,7 +2032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -2068,7 +2068,7 @@
         <v>167494</v>
       </c>
     </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -2104,7 +2104,7 @@
         <v>960.3</v>
       </c>
     </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -2140,7 +2140,7 @@
         <v>174.41</v>
       </c>
     </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -2176,7 +2176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -2212,7 +2212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -2286,7 +2286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -2322,7 +2322,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -2358,7 +2358,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -2394,7 +2394,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -2466,7 +2466,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -2502,7 +2502,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -2538,7 +2538,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -2574,7 +2574,7 @@
         <v>510544</v>
       </c>
     </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -2610,7 +2610,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -2646,7 +2646,7 @@
         <v>531.59</v>
       </c>
     </row>
-    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -2682,7 +2682,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -2718,7 +2718,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -2792,7 +2792,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -2828,7 +2828,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -2864,7 +2864,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -2900,7 +2900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -2972,7 +2972,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -3008,7 +3008,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -3044,7 +3044,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -3080,7 +3080,7 @@
         <v>521958</v>
       </c>
     </row>
-    <row r="47" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -3116,7 +3116,7 @@
         <v>960.8</v>
       </c>
     </row>
-    <row r="48" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -3152,7 +3152,7 @@
         <v>543.26</v>
       </c>
     </row>
-    <row r="49" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -3188,7 +3188,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:18" x14ac:dyDescent="0.35">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -3243,14 +3243,14 @@
       <selection activeCell="L16" sqref="L16:L50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
     <col min="7" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>158</v>
       </c>
@@ -3261,7 +3261,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -3328,7 +3328,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -3349,7 +3349,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -3370,7 +3370,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -3391,7 +3391,7 @@
         <v>1.81</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -3412,7 +3412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -3433,7 +3433,7 @@
         <v>42.68</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -3454,7 +3454,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -3475,7 +3475,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -3496,7 +3496,7 @@
         <v>83926</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -3517,7 +3517,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -3538,7 +3538,7 @@
         <v>87.42</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -3559,7 +3559,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -3580,7 +3580,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -3624,7 +3624,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -3645,7 +3645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -3666,7 +3666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -3687,7 +3687,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -3708,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -3729,7 +3729,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -3750,7 +3750,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -3771,7 +3771,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -3792,7 +3792,7 @@
         <v>839084</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -3813,7 +3813,7 @@
         <v>960.7</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -3834,7 +3834,7 @@
         <v>873.39</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -3855,7 +3855,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -3876,7 +3876,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -3920,7 +3920,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -3941,7 +3941,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -3962,7 +3962,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -3983,7 +3983,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -4004,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -4025,7 +4025,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -4046,7 +4046,7 @@
         <v>692.49</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -4067,7 +4067,7 @@
         <v>702.28</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -4088,7 +4088,7 @@
         <v>2129167</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -4109,7 +4109,7 @@
         <v>960.8</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -4130,7 +4130,7 @@
         <v>2216.09</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -4151,7 +4151,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -4187,19 +4187,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FCC0AA-C984-4903-81D8-D871D2663DA5}">
   <dimension ref="E7:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
     <col min="7" max="11" width="9" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
@@ -4210,7 +4210,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -4277,7 +4277,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -4298,7 +4298,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -4319,7 +4319,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -4340,7 +4340,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -4361,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -4382,7 +4382,7 @@
         <v>43.13</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -4403,7 +4403,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -4424,7 +4424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -4445,7 +4445,7 @@
         <v>83888</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -4466,7 +4466,7 @@
         <v>960.6</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -4487,7 +4487,7 @@
         <v>87.33</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -4508,7 +4508,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -4529,7 +4529,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -4573,7 +4573,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -4594,7 +4594,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -4615,7 +4615,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -4636,7 +4636,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -4657,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -4678,7 +4678,7 @@
         <v>142.69999999999999</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -4699,7 +4699,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -4720,7 +4720,7 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -4741,7 +4741,7 @@
         <v>838800</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -4762,7 +4762,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -4783,7 +4783,7 @@
         <v>873.34</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -4804,7 +4804,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -4825,7 +4825,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -4869,7 +4869,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -4890,7 +4890,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -4911,7 +4911,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -4932,7 +4932,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -4953,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -4974,7 +4974,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -4995,7 +4995,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -5016,7 +5016,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -5037,7 +5037,7 @@
         <v>1642210</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -5058,7 +5058,7 @@
         <v>960.6</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -5079,7 +5079,7 @@
         <v>1709.57</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -5100,7 +5100,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -5137,18 +5137,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33E3BDB-BD67-41A1-991C-2FB34B0212C5}">
   <dimension ref="E7:K50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
     <col min="7" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>72</v>
       </c>
@@ -5159,7 +5159,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -5226,7 +5226,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -5247,7 +5247,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -5268,7 +5268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -5289,7 +5289,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -5310,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -5331,7 +5331,7 @@
         <v>42.53</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -5352,7 +5352,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -5373,7 +5373,7 @@
         <v>3.92</v>
       </c>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -5394,7 +5394,7 @@
         <v>83889</v>
       </c>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -5415,7 +5415,7 @@
         <v>960.5</v>
       </c>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -5436,7 +5436,7 @@
         <v>87.34</v>
       </c>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -5457,7 +5457,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -5478,7 +5478,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -5522,7 +5522,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -5543,7 +5543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -5564,7 +5564,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -5585,7 +5585,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -5606,7 +5606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -5627,7 +5627,7 @@
         <v>42.03</v>
       </c>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -5648,7 +5648,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -5669,7 +5669,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -5690,7 +5690,7 @@
         <v>838747</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -5711,7 +5711,7 @@
         <v>960.4</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -5732,7 +5732,7 @@
         <v>873.32</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -5753,7 +5753,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -5774,7 +5774,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -5818,7 +5818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -5839,7 +5839,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -5860,7 +5860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -5881,7 +5881,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -5902,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -5923,7 +5923,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -5944,7 +5944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -5965,7 +5965,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -5986,7 +5986,7 @@
         <v>1707670</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -6007,7 +6007,7 @@
         <v>960.5</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -6028,7 +6028,7 @@
         <v>1777.84</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -6049,7 +6049,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>
@@ -6086,18 +6086,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE1C407F-A9FB-4106-8CC9-34E1EF3B9F3E}">
   <dimension ref="E7:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
     <col min="7" max="11" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E7" s="5" t="s">
         <v>72</v>
       </c>
@@ -6108,7 +6108,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E9" s="8">
         <v>100</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="1" t="s">
         <v>14</v>
@@ -6175,7 +6175,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
@@ -6196,7 +6196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="1" t="s">
         <v>16</v>
@@ -6217,7 +6217,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="1" t="s">
         <v>1</v>
@@ -6238,7 +6238,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -6259,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="1" t="s">
         <v>3</v>
@@ -6280,7 +6280,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="1" t="s">
         <v>4</v>
@@ -6301,7 +6301,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="1" t="s">
         <v>5</v>
@@ -6322,7 +6322,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="1" t="s">
         <v>6</v>
@@ -6347,7 +6347,7 @@
         <v>83902.399999999994</v>
       </c>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="1" t="s">
         <v>7</v>
@@ -6372,7 +6372,7 @@
         <v>960.41999999999985</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -6397,7 +6397,7 @@
         <v>87.36</v>
       </c>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -6418,7 +6418,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E22" s="10"/>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -6439,7 +6439,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E23" s="8">
         <v>1000</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
         <v>14</v>
@@ -6483,7 +6483,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -6504,7 +6504,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="2" t="s">
         <v>16</v>
@@ -6525,7 +6525,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
         <v>1</v>
@@ -6546,7 +6546,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
         <v>2</v>
@@ -6567,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
         <v>3</v>
@@ -6588,7 +6588,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
         <v>4</v>
@@ -6609,7 +6609,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
         <v>5</v>
@@ -6630,7 +6630,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
@@ -6655,7 +6655,7 @@
         <v>838855.6</v>
       </c>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
         <v>7</v>
@@ -6680,7 +6680,7 @@
         <v>960.78000000000009</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -6705,7 +6705,7 @@
         <v>873.1</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -6726,7 +6726,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E36" s="10"/>
       <c r="F36" s="2" t="s">
         <v>9</v>
@@ -6747,7 +6747,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E37" s="8">
         <v>4000</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="1" t="s">
         <v>14</v>
@@ -6791,7 +6791,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -6812,7 +6812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -6833,7 +6833,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -6854,7 +6854,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="1" t="s">
         <v>2</v>
@@ -6875,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>3</v>
@@ -6896,7 +6896,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="1" t="s">
         <v>4</v>
@@ -6921,7 +6921,7 @@
         <v>958.87599999999998</v>
       </c>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="1" t="s">
         <v>5</v>
@@ -6946,7 +6946,7 @@
         <v>970.31799999999998</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="1" t="s">
         <v>6</v>
@@ -6971,7 +6971,7 @@
         <v>1860542.4</v>
       </c>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="1" t="s">
         <v>7</v>
@@ -6996,7 +6996,7 @@
         <v>960.72</v>
       </c>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
         <v>8</v>
@@ -7021,7 +7021,7 @@
         <v>1936.5960000000002</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="1" t="s">
         <v>11</v>
@@ -7042,7 +7042,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="10"/>
       <c r="F50" s="1" t="s">
         <v>9</v>

</xml_diff>